<commit_message>
Refactor, hamcrest and division of features
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcgomez\IdeaProjects\GUIChallenge\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53FF06AF-4458-4694-BFB5-80FABE866854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2E24D4C-FAB1-4DD2-B9C3-952F1CE0C3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="480" windowWidth="27015" windowHeight="14010" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="27015" windowHeight="14010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidCredentials" sheetId="1" r:id="rId1"/>
     <sheet name="Genre" sheetId="2" r:id="rId2"/>
     <sheet name="Filter" sheetId="3" r:id="rId3"/>
+    <sheet name="Movies" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>username</t>
   </si>
@@ -54,6 +55,12 @@
   </si>
   <si>
     <t>number of dates</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Fight Club</t>
   </si>
 </sst>
 </file>
@@ -442,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B7C064A-8DD2-426F-ADA7-27CECE4B07CF}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
@@ -472,4 +479,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A428231F-84AE-4273-9B27-404DF2F7BB45}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>